<commit_message>
Working on functions to do the combined analysis with the 2020/2021 data
</commit_message>
<xml_diff>
--- a/exports/lsmean_files/Jay Test 2 - LSMeans.xlsx
+++ b/exports/lsmean_files/Jay Test 2 - LSMeans.xlsx
@@ -784,13 +784,13 @@
         <v>40.6</v>
       </c>
       <c r="Y5" s="1" t="n">
-        <v>63.1</v>
+        <v>63</v>
       </c>
       <c r="Z5" s="1" t="n">
         <v>12</v>
       </c>
       <c r="AA5" s="1" t="n">
-        <v>54.8</v>
+        <v>54.9</v>
       </c>
       <c r="AB5" s="1" t="n">
         <v>1692.7</v>
@@ -1113,7 +1113,7 @@
         <v>2016.6</v>
       </c>
       <c r="T9" s="1" t="n">
-        <v>33.7</v>
+        <v>33.8</v>
       </c>
       <c r="U9" s="1" t="n">
         <v>1.9</v>
@@ -1137,7 +1137,7 @@
         <v>57.6</v>
       </c>
       <c r="AB9" s="1" t="n">
-        <v>2266.1</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="10">
@@ -1199,7 +1199,7 @@
         <v>2032</v>
       </c>
       <c r="T10" s="1" t="n">
-        <v>31.7</v>
+        <v>31.8</v>
       </c>
       <c r="U10" s="1" t="n">
         <v>1.9</v>
@@ -1285,7 +1285,7 @@
         <v>2003.8</v>
       </c>
       <c r="T11" s="1" t="n">
-        <v>32.7</v>
+        <v>32.8</v>
       </c>
       <c r="U11" s="1" t="n">
         <v>1.5</v>
@@ -1371,7 +1371,7 @@
         <v>1979.6</v>
       </c>
       <c r="T12" s="1" t="n">
-        <v>33.2</v>
+        <v>33.3</v>
       </c>
       <c r="U12" s="1" t="n">
         <v>1.9</v>
@@ -1543,7 +1543,7 @@
         <v>1485.8</v>
       </c>
       <c r="T14" s="1" t="n">
-        <v>37.7</v>
+        <v>37.8</v>
       </c>
       <c r="U14" s="1" t="n">
         <v>2.3</v>
@@ -1715,7 +1715,7 @@
         <v>1925</v>
       </c>
       <c r="T16" s="1" t="n">
-        <v>34.7</v>
+        <v>34.8</v>
       </c>
       <c r="U16" s="1" t="n">
         <v>1.3</v>
@@ -1887,7 +1887,7 @@
         <v>2078.1</v>
       </c>
       <c r="T18" s="1" t="n">
-        <v>31.7</v>
+        <v>31.8</v>
       </c>
       <c r="U18" s="1" t="n">
         <v>1.5</v>
@@ -1973,7 +1973,7 @@
         <v>1821.6</v>
       </c>
       <c r="T19" s="1" t="n">
-        <v>31.2</v>
+        <v>31.3</v>
       </c>
       <c r="U19" s="1" t="n">
         <v>1.3</v>
@@ -2047,7 +2047,7 @@
         <v>45.8</v>
       </c>
       <c r="P20" s="1" t="n">
-        <v>67.2</v>
+        <v>67.1</v>
       </c>
       <c r="Q20" s="1" t="n">
         <v>12.7</v>
@@ -2145,7 +2145,7 @@
         <v>2032.2</v>
       </c>
       <c r="T21" s="1" t="n">
-        <v>36.7</v>
+        <v>36.8</v>
       </c>
       <c r="U21" s="1" t="n">
         <v>2</v>
@@ -2225,13 +2225,13 @@
         <v>13.4</v>
       </c>
       <c r="R22" s="1" t="n">
-        <v>57.4</v>
+        <v>57.5</v>
       </c>
       <c r="S22" s="1" t="n">
         <v>2067.8</v>
       </c>
       <c r="T22" s="1" t="n">
-        <v>35.7</v>
+        <v>35.8</v>
       </c>
       <c r="U22" s="1" t="n">
         <v>1.5</v>
@@ -2252,7 +2252,7 @@
         <v>14.6</v>
       </c>
       <c r="AA22" s="1" t="n">
-        <v>57</v>
+        <v>57.1</v>
       </c>
       <c r="AB22" s="1" t="n">
         <v>2304.4</v>

</xml_diff>